<commit_message>
Rewrite the plan of the iteration
</commit_message>
<xml_diff>
--- a/Documents/IterationPlan.xlsx
+++ b/Documents/IterationPlan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
   <si>
     <t>Product</t>
   </si>
@@ -250,12 +250,6 @@
     <t>Sunday,09/09/2018</t>
   </si>
   <si>
-    <t>Monday,10/09/2018</t>
-  </si>
-  <si>
-    <t>Sunday,16/09/2018</t>
-  </si>
-  <si>
     <t>Monday,06/08/2018</t>
   </si>
   <si>
@@ -269,9 +263,6 @@
   </si>
   <si>
     <t>Monday,08/10/2018</t>
-  </si>
-  <si>
-    <t>StuVac</t>
   </si>
   <si>
     <t>Sunday,23/09/2018</t>
@@ -297,7 +288,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,12 +323,6 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -417,12 +402,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -453,7 +432,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="38887.738159722219" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="277">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:D6" sheet="Source Data"/>
+    <worksheetSource ref="B1:D9" sheet="Source Data"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Product" numFmtId="0">
@@ -3755,7 +3734,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,10 +3772,10 @@
         <v>49</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
@@ -3854,18 +3833,6 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="E6" s="8">
         <v>1</v>
       </c>
@@ -3891,17 +3858,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>81</v>
+      <c r="A9" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" s="8">
         <v>2</v>
@@ -3915,10 +3882,10 @@
         <v>52</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E10" s="8">
         <v>2</v>
@@ -3932,10 +3899,10 @@
         <v>53</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E11" s="8">
         <v>2</v>
@@ -3949,10 +3916,10 @@
         <v>63</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E12" s="8">
         <v>2</v>
@@ -3966,10 +3933,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E13" s="8">
         <v>2</v>

</xml_diff>

<commit_message>
Update the plan and schedual
</commit_message>
<xml_diff>
--- a/Documents/IterationPlan.xlsx
+++ b/Documents/IterationPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\我的文档\桌面\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Homework\SEP\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="8745"/>
   </bookViews>
   <sheets>
     <sheet name="Source Data" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="By Product-Customer" sheetId="7" r:id="rId3"/>
     <sheet name="By Product-Customer Filtered" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="87">
   <si>
     <t>Product</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>Sunday,14/10/2018</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>Monday,15/10/2018</t>
+  </si>
+  <si>
+    <t>Sunday,22/10/2018</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="38887.738159722219" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="277">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:D9" sheet="Source Data"/>
+    <worksheetSource ref="B1:D8" sheet="Source Data"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Product" numFmtId="0">
@@ -3734,7 +3743,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3833,6 +3842,18 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="E6" s="8">
         <v>1</v>
       </c>
@@ -3859,16 +3880,16 @@
     </row>
     <row r="9" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E9" s="8">
         <v>2</v>
@@ -3876,16 +3897,16 @@
     </row>
     <row r="10" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E10" s="8">
         <v>2</v>
@@ -3893,16 +3914,16 @@
     </row>
     <row r="11" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E11" s="8">
         <v>2</v>
@@ -3910,16 +3931,16 @@
     </row>
     <row r="12" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E12" s="8">
         <v>2</v>
@@ -3927,16 +3948,16 @@
     </row>
     <row r="13" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E13" s="8">
         <v>2</v>

</xml_diff>